<commit_message>
Add patient table for batch 2
</commit_message>
<xml_diff>
--- a/tables/patient_table_batch2_5_patients.xlsx
+++ b/tables/patient_table_batch2_5_patients.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="28">
   <si>
     <t xml:space="preserve">patient</t>
   </si>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">condition</t>
   </si>
   <si>
+    <t xml:space="preserve">ever_smoker</t>
+  </si>
+  <si>
     <t xml:space="preserve">P4</t>
   </si>
   <si>
@@ -61,6 +64,9 @@
     <t xml:space="preserve">LUAD</t>
   </si>
   <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
     <t xml:space="preserve">tumor_primary</t>
   </si>
   <si>
@@ -70,6 +76,9 @@
     <t xml:space="preserve">LCBio_02</t>
   </si>
   <si>
+    <t xml:space="preserve">II</t>
+  </si>
+  <si>
     <t xml:space="preserve">P6</t>
   </si>
   <si>
@@ -79,9 +88,6 @@
     <t xml:space="preserve">male</t>
   </si>
   <si>
-    <t xml:space="preserve">II</t>
-  </si>
-  <si>
     <t xml:space="preserve">LSCC</t>
   </si>
   <si>
@@ -89,6 +95,9 @@
   </si>
   <si>
     <t xml:space="preserve">LCBio_04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">III</t>
   </si>
   <si>
     <t xml:space="preserve">P8</t>
@@ -101,9 +110,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -187,17 +195,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -232,10 +236,10 @@
   <dimension ref="A1:AMJ20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.83"/>
@@ -243,11 +247,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="0" width="10.5"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -269,8 +274,10 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3"/>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2"/>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
@@ -279,269 +286,311 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>61</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>61</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>62</v>
       </c>
+      <c r="F4" s="0" t="s">
+        <v>18</v>
+      </c>
       <c r="G4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>62</v>
       </c>
+      <c r="F5" s="0" t="s">
+        <v>18</v>
+      </c>
       <c r="G5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>72</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>72</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>69</v>
       </c>
+      <c r="F8" s="0" t="s">
+        <v>25</v>
+      </c>
       <c r="G8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>69</v>
       </c>
+      <c r="F9" s="0" t="s">
+        <v>25</v>
+      </c>
       <c r="G9" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>67</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>67</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="G15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="G16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="G17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="G18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="G20" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>